<commit_message>
All curve data read from JS
</commit_message>
<xml_diff>
--- a/PCI/Airfield_AC_Curve.xlsx
+++ b/PCI/Airfield_AC_Curve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VS_PCI\PCI\PCI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD12EE14-02EF-4020-AC36-10153126DD56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79799C30-67CC-48BC-AD02-078A50BEA997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="16" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-Alligator cracking" sheetId="3" r:id="rId1"/>
@@ -497,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED90409E-9100-41B3-983A-D377F2118842}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,8 +1062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2349783-1006-4200-9A90-241EF2A7A8B8}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection sqref="A1:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1905,7 +1905,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3589,7 +3589,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection sqref="A1:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4009,7 +4009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{874CE120-9832-4917-91CF-544B85AD4B41}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection sqref="A1:D29"/>
     </sheetView>
   </sheetViews>
@@ -4430,8 +4430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08930E69-A74F-4814-A7FF-2E6532DAB3B7}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4851,8 +4851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB669D6-13CE-48AF-9671-EDF3021688CA}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection sqref="A1:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5272,7 +5272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D451432-809F-4E8B-A090-427CA6D2220A}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection sqref="A1:D29"/>
     </sheetView>
   </sheetViews>
@@ -6115,7 +6115,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection sqref="A1:K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7252,8 +7252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF83AF0B-DE12-4716-B1CB-C5D0648D0827}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection sqref="A1:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>